<commit_message>
Solucion de comentarios realiados por el area de conocimiento se realiza la separacion de feature y se modifica los pasos que se tenian en el pageobject
</commit_message>
<xml_diff>
--- a/retoLibreria.xlsx
+++ b/retoLibreria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automatizacion\RetoLibreriaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CFA2A3-CC7C-4AE4-913F-31A6A1C93BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A7892E-8273-4CFF-837E-1A4E717C052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B9F01DF8-C618-4471-930E-1729E2CEA87F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{B9F01DF8-C618-4471-930E-1729E2CEA87F}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoBasica" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
     <t>MEDELLIN</t>
   </si>
   <si>
-    <t>pruebareto01@yopmail.com</t>
+    <t>pruebareto1001@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414D9DE2-6BB3-4837-845B-364527CD1154}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28749D78-7134-4F19-BB9D-2402217C5415}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambio de versionamiento de dependencias y data en archivo de excel
</commit_message>
<xml_diff>
--- a/retoLibreria.xlsx
+++ b/retoLibreria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automatizacion\RetoLibreriaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A7892E-8273-4CFF-837E-1A4E717C052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F320B3F6-D9F6-483E-AFAE-2E26C243FF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{B9F01DF8-C618-4471-930E-1729E2CEA87F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B9F01DF8-C618-4471-930E-1729E2CEA87F}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoBasica" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
     <t>MEDELLIN</t>
   </si>
   <si>
-    <t>pruebareto1001@yopmail.com</t>
+    <t>pruebareto1111@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414D9DE2-6BB3-4837-845B-364527CD1154}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28749D78-7134-4F19-BB9D-2402217C5415}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>